<commit_message>
Finalização da Documentação, Diagrama de Negócio e Diagrama de Solução Técnica feitos.
</commit_message>
<xml_diff>
--- a/Documentos/Product-Backlog.xlsx
+++ b/Documentos/Product-Backlog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zdusa\OneDrive\Documentos\ZDU\SPTECH ZDU\1° Semestre\Projeto-Individual\Documentos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D9F2E1D-6D53-41B5-9265-66EC7688A04D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F85BA542-3C0C-4B8A-B1E7-B393765BE7D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -104,9 +104,6 @@
     <t>Contexto, Objetivo, Justificativa e Escopo (Descrição resumida do projeto, Requisitos do Projeto, Macro Cronograma, Riscos e Restrições, Resultados Esperado, Limites e Exclusões, Recursos Necessários, Partes interessadas (stakeholders)</t>
   </si>
   <si>
-    <t>Desenvolver uma narrativa coerente do porque o tema (Criação de jogos) é imporante para mim.</t>
-  </si>
-  <si>
     <t>Tela de Cadastro</t>
   </si>
   <si>
@@ -602,6 +599,9 @@
   </si>
   <si>
     <t>Criar a identidade visual tanto do site como do jogo</t>
+  </si>
+  <si>
+    <t>Desenvolver uma narrativa coerente do porque o tema (Criação de jogos) é importante para mim.</t>
   </si>
 </sst>
 </file>
@@ -1276,6 +1276,9 @@
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>315</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>284</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2352,7 +2355,7 @@
   <dimension ref="A1:M44"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="I26" sqref="I26"/>
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2380,7 +2383,7 @@
       <c r="F1" s="62"/>
       <c r="G1" s="62"/>
       <c r="I1" s="61" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="J1" s="61"/>
       <c r="K1" s="61"/>
@@ -2411,22 +2414,22 @@
       </c>
       <c r="I2" s="32"/>
       <c r="J2" s="33" t="s">
+        <v>91</v>
+      </c>
+      <c r="K2" s="33" t="s">
         <v>92</v>
       </c>
-      <c r="K2" s="33" t="s">
+      <c r="L2" s="33" t="s">
         <v>93</v>
       </c>
-      <c r="L2" s="33" t="s">
+      <c r="M2" s="33" t="s">
         <v>94</v>
-      </c>
-      <c r="M2" s="33" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="38"/>
       <c r="B3" s="37" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C3" s="39"/>
       <c r="D3" s="39"/>
@@ -2434,7 +2437,7 @@
       <c r="F3" s="39"/>
       <c r="G3" s="40"/>
       <c r="I3" s="31" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="J3" s="1">
         <f>SUM(E4:E5,E7:E17,E19:E25,E27:E38,E40:E44)</f>
@@ -2442,7 +2445,7 @@
       </c>
       <c r="K3" s="1">
         <f>SUM(K4:K8)</f>
-        <v>13</v>
+        <v>44</v>
       </c>
       <c r="L3" s="1">
         <f>J3</f>
@@ -2464,7 +2467,7 @@
         <v>8</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E4" s="5">
         <v>5</v>
@@ -2473,10 +2476,10 @@
         <v>2</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="I4" s="32" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J4" s="1">
         <f>SUM(E4:E5)</f>
@@ -2505,7 +2508,7 @@
         <v>8</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E5" s="5">
         <v>8</v>
@@ -2514,28 +2517,31 @@
         <v>1</v>
       </c>
       <c r="G5" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="I5" s="32" t="s">
         <v>83</v>
-      </c>
-      <c r="I5" s="32" t="s">
-        <v>84</v>
       </c>
       <c r="J5" s="1">
         <f>SUM(E7:E17)</f>
         <v>102</v>
       </c>
       <c r="K5" s="1">
-        <v>0</v>
+        <v>31</v>
       </c>
       <c r="L5" s="1">
         <f>L4-J5</f>
         <v>213</v>
       </c>
-      <c r="M5" s="1"/>
+      <c r="M5" s="1">
+        <f>M4-K5</f>
+        <v>284</v>
+      </c>
     </row>
     <row r="6" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="35"/>
       <c r="B6" s="34" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C6" s="35"/>
       <c r="D6" s="35"/>
@@ -2543,7 +2549,7 @@
       <c r="F6" s="35"/>
       <c r="G6" s="36"/>
       <c r="I6" s="32" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="J6" s="1">
         <f>SUM(E19:E25)</f>
@@ -2566,10 +2572,10 @@
         <v>20</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E7" s="8">
         <v>21</v>
@@ -2578,10 +2584,10 @@
         <v>1</v>
       </c>
       <c r="G7" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="I7" s="32" t="s">
         <v>84</v>
-      </c>
-      <c r="I7" s="32" t="s">
-        <v>85</v>
       </c>
       <c r="J7" s="1">
         <f>SUM(E27:E38)</f>
@@ -2598,16 +2604,16 @@
     </row>
     <row r="8" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="27" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C8" s="7" t="s">
         <v>8</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E8" s="8">
         <v>5</v>
@@ -2616,10 +2622,10 @@
         <v>10</v>
       </c>
       <c r="G8" s="8" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I8" s="32" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="J8" s="1">
         <f>SUM(E40:E44)</f>
@@ -2636,16 +2642,16 @@
     </row>
     <row r="9" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="28" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C9" s="7" t="s">
         <v>8</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E9" s="8">
         <v>5</v>
@@ -2654,7 +2660,7 @@
         <v>9</v>
       </c>
       <c r="G9" s="8" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="10" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
@@ -2662,13 +2668,13 @@
         <v>17</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>21</v>
+        <v>100</v>
       </c>
       <c r="C10" s="7" t="s">
         <v>8</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E10" s="8">
         <v>13</v>
@@ -2677,21 +2683,21 @@
         <v>2</v>
       </c>
       <c r="G10" s="8" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="11" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="28" t="s">
+        <v>98</v>
+      </c>
+      <c r="B11" s="9" t="s">
         <v>99</v>
-      </c>
-      <c r="B11" s="9" t="s">
-        <v>100</v>
       </c>
       <c r="C11" s="7" t="s">
         <v>8</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E11" s="8">
         <v>3</v>
@@ -2700,21 +2706,21 @@
         <v>11</v>
       </c>
       <c r="G11" s="8" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="12" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C12" s="7" t="s">
         <v>8</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E12" s="8">
         <v>8</v>
@@ -2723,21 +2729,21 @@
         <v>3</v>
       </c>
       <c r="G12" s="8" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="13" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C13" s="7" t="s">
         <v>8</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E13" s="8">
         <v>5</v>
@@ -2746,21 +2752,21 @@
         <v>4</v>
       </c>
       <c r="G13" s="8" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="14" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C14" s="7" t="s">
         <v>8</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E14" s="8">
         <v>5</v>
@@ -2769,21 +2775,21 @@
         <v>5</v>
       </c>
       <c r="G14" s="8" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="15" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="10" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C15" s="7" t="s">
         <v>8</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E15" s="8">
         <v>8</v>
@@ -2792,21 +2798,21 @@
         <v>8</v>
       </c>
       <c r="G15" s="8" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="16" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C16" s="7" t="s">
         <v>8</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E16" s="8">
         <v>8</v>
@@ -2815,7 +2821,7 @@
         <v>7</v>
       </c>
       <c r="G16" s="8" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
@@ -2823,13 +2829,13 @@
         <v>12</v>
       </c>
       <c r="B17" s="55" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E17" s="8">
         <v>21</v>
@@ -2838,13 +2844,13 @@
         <v>6</v>
       </c>
       <c r="G17" s="8" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="42"/>
       <c r="B18" s="41" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C18" s="43"/>
       <c r="D18" s="43"/>
@@ -2854,16 +2860,16 @@
     </row>
     <row r="19" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B19" s="56" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C19" s="13" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D19" s="14" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E19" s="14">
         <v>8</v>
@@ -2872,21 +2878,21 @@
         <v>1</v>
       </c>
       <c r="G19" s="14" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="11" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B20" s="12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C20" s="13" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D20" s="14" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E20" s="14">
         <v>8</v>
@@ -2895,7 +2901,7 @@
         <v>2</v>
       </c>
       <c r="G20" s="14" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
@@ -2903,13 +2909,13 @@
         <v>13</v>
       </c>
       <c r="B21" s="15" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C21" s="13" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D21" s="14" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E21" s="14">
         <v>8</v>
@@ -2918,21 +2924,21 @@
         <v>3</v>
       </c>
       <c r="G21" s="14" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="11" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B22" s="16" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C22" s="13" t="s">
         <v>8</v>
       </c>
       <c r="D22" s="14" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E22" s="14">
         <v>5</v>
@@ -2941,21 +2947,21 @@
         <v>4</v>
       </c>
       <c r="G22" s="14" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" s="11" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B23" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="C23" s="13" t="s">
         <v>74</v>
       </c>
-      <c r="C23" s="13" t="s">
-        <v>75</v>
-      </c>
       <c r="D23" s="14" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E23" s="14">
         <v>5</v>
@@ -2964,21 +2970,21 @@
         <v>5</v>
       </c>
       <c r="G23" s="14" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="11" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B24" s="16" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C24" s="13" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D24" s="14" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E24" s="14">
         <v>8</v>
@@ -2987,21 +2993,21 @@
         <v>6</v>
       </c>
       <c r="G24" s="14" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="11" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B25" s="57" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C25" s="13" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D25" s="14" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E25" s="14">
         <v>13</v>
@@ -3010,13 +3016,13 @@
         <v>7</v>
       </c>
       <c r="G25" s="14" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="46"/>
       <c r="B26" s="45" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C26" s="47"/>
       <c r="D26" s="47"/>
@@ -3029,13 +3035,13 @@
         <v>16</v>
       </c>
       <c r="B27" s="58" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C27" s="22" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D27" s="23" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E27" s="23">
         <v>13</v>
@@ -3044,21 +3050,21 @@
         <v>4</v>
       </c>
       <c r="G27" s="23" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A28" s="24" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B28" s="21" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C28" s="22" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D28" s="23" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E28" s="23">
         <v>8</v>
@@ -3067,21 +3073,21 @@
         <v>5</v>
       </c>
       <c r="G28" s="23" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A29" s="24" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B29" s="21" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C29" s="22" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D29" s="23" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E29" s="23">
         <v>8</v>
@@ -3090,21 +3096,21 @@
         <v>6</v>
       </c>
       <c r="G29" s="23" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A30" s="24" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B30" s="25" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C30" s="22" t="s">
         <v>8</v>
       </c>
       <c r="D30" s="23" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E30" s="23">
         <v>8</v>
@@ -3113,21 +3119,21 @@
         <v>8</v>
       </c>
       <c r="G30" s="23" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A31" s="24" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B31" s="25" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C31" s="22" t="s">
         <v>8</v>
       </c>
       <c r="D31" s="23" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E31" s="23">
         <v>8</v>
@@ -3136,21 +3142,21 @@
         <v>9</v>
       </c>
       <c r="G31" s="23" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="32" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A32" s="24" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B32" s="25" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C32" s="22" t="s">
         <v>8</v>
       </c>
       <c r="D32" s="23" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E32" s="23">
         <v>21</v>
@@ -3159,21 +3165,21 @@
         <v>10</v>
       </c>
       <c r="G32" s="23" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="33" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A33" s="24" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B33" s="25" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C33" s="22" t="s">
         <v>8</v>
       </c>
       <c r="D33" s="23" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E33" s="23">
         <v>21</v>
@@ -3182,21 +3188,21 @@
         <v>11</v>
       </c>
       <c r="G33" s="23" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="34" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A34" s="30" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B34" s="21" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C34" s="22" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D34" s="23" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E34" s="23">
         <v>8</v>
@@ -3205,7 +3211,7 @@
         <v>1</v>
       </c>
       <c r="G34" s="23" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="35" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
@@ -3213,13 +3219,13 @@
         <v>11</v>
       </c>
       <c r="B35" s="21" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C35" s="22" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D35" s="23" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E35" s="23">
         <v>5</v>
@@ -3228,7 +3234,7 @@
         <v>2</v>
       </c>
       <c r="G35" s="23" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="36" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
@@ -3236,13 +3242,13 @@
         <v>14</v>
       </c>
       <c r="B36" s="21" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C36" s="22" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D36" s="23" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E36" s="23">
         <v>5</v>
@@ -3251,21 +3257,21 @@
         <v>3</v>
       </c>
       <c r="G36" s="23" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="37" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A37" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="B37" s="21" t="s">
         <v>63</v>
       </c>
-      <c r="B37" s="21" t="s">
-        <v>64</v>
-      </c>
       <c r="C37" s="22" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D37" s="23" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E37" s="23">
         <v>8</v>
@@ -3274,21 +3280,21 @@
         <v>7</v>
       </c>
       <c r="G37" s="23" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="38" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A38" s="24" t="s">
+        <v>89</v>
+      </c>
+      <c r="B38" s="59" t="s">
         <v>90</v>
       </c>
-      <c r="B38" s="59" t="s">
-        <v>91</v>
-      </c>
       <c r="C38" s="22" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D38" s="23" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E38" s="23">
         <v>8</v>
@@ -3297,13 +3303,13 @@
         <v>12</v>
       </c>
       <c r="G38" s="23" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="39" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A39" s="50"/>
       <c r="B39" s="49" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C39" s="51"/>
       <c r="D39" s="51"/>
@@ -3313,16 +3319,16 @@
     </row>
     <row r="40" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A40" s="17" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B40" s="60" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C40" s="19" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D40" s="20" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E40" s="20">
         <v>5</v>
@@ -3331,21 +3337,21 @@
         <v>3</v>
       </c>
       <c r="G40" s="20" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="41" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A41" s="17" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B41" s="18" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C41" s="19" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D41" s="20" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E41" s="20">
         <v>5</v>
@@ -3354,21 +3360,21 @@
         <v>4</v>
       </c>
       <c r="G41" s="20" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="42" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A42" s="17" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B42" s="18" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C42" s="19" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D42" s="20" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E42" s="20">
         <v>3</v>
@@ -3377,21 +3383,21 @@
         <v>1</v>
       </c>
       <c r="G42" s="20" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="43" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A43" s="17" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B43" s="18" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C43" s="19" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D43" s="20" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E43" s="20">
         <v>3</v>
@@ -3400,21 +3406,21 @@
         <v>2</v>
       </c>
       <c r="G43" s="20" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="44" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A44" s="17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B44" s="18" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C44" s="19" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D44" s="20" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E44" s="20">
         <v>21</v>
@@ -3423,7 +3429,7 @@
         <v>5</v>
       </c>
       <c r="G44" s="20" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Começando o protótipo do site, + paleta de cores/identidade visual definida.
</commit_message>
<xml_diff>
--- a/Documentos/Product-Backlog.xlsx
+++ b/Documentos/Product-Backlog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zdusa\OneDrive\Documentos\ZDU\SPTECH ZDU\1° Semestre\Projeto-Individual\Documentos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F85BA542-3C0C-4B8A-B1E7-B393765BE7D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A6FD9DE-CED3-4217-A239-10EE9791B37D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1278,7 +1278,7 @@
                   <c:v>315</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>284</c:v>
+                  <c:v>281</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2355,7 +2355,7 @@
   <dimension ref="A1:M44"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+      <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2445,7 +2445,7 @@
       </c>
       <c r="K3" s="1">
         <f>SUM(K4:K8)</f>
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="L3" s="1">
         <f>J3</f>
@@ -2527,7 +2527,7 @@
         <v>102</v>
       </c>
       <c r="K5" s="1">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="L5" s="1">
         <f>L4-J5</f>
@@ -2535,7 +2535,7 @@
       </c>
       <c r="M5" s="1">
         <f>M4-K5</f>
-        <v>284</v>
+        <v>281</v>
       </c>
     </row>
     <row r="6" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Tentando resolver o b.0
</commit_message>
<xml_diff>
--- a/Documentos/Product-Backlog.xlsx
+++ b/Documentos/Product-Backlog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zdusa\OneDrive\Documentos\ZDU\SPTECH ZDU\1° Semestre\Projeto-Individual\Documentos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A6FD9DE-CED3-4217-A239-10EE9791B37D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{161A4312-529B-4E5F-9B7B-5B1EA32F0D6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1278,7 +1278,10 @@
                   <c:v>315</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>281</c:v>
+                  <c:v>284</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>263</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2355,7 +2358,7 @@
   <dimension ref="A1:M44"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2445,7 +2448,7 @@
       </c>
       <c r="K3" s="1">
         <f>SUM(K4:K8)</f>
-        <v>47</v>
+        <v>65</v>
       </c>
       <c r="L3" s="1">
         <f>J3</f>
@@ -2527,7 +2530,7 @@
         <v>102</v>
       </c>
       <c r="K5" s="1">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="L5" s="1">
         <f>L4-J5</f>
@@ -2535,7 +2538,7 @@
       </c>
       <c r="M5" s="1">
         <f>M4-K5</f>
-        <v>281</v>
+        <v>284</v>
       </c>
     </row>
     <row r="6" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2556,13 +2559,16 @@
         <v>55</v>
       </c>
       <c r="K6" s="1">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="L6" s="1">
         <f>L5-J6</f>
         <v>158</v>
       </c>
-      <c r="M6" s="1"/>
+      <c r="M6" s="1">
+        <f>M5-K6</f>
+        <v>263</v>
+      </c>
     </row>
     <row r="7" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="27" t="s">

</xml_diff>

<commit_message>
Atualização do backlog e gráfico de Burndown.
</commit_message>
<xml_diff>
--- a/Documentos/Product-Backlog.xlsx
+++ b/Documentos/Product-Backlog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zdusa\OneDrive\Documentos\ZDU\SPTECH ZDU\1° Semestre\Projeto-Individual\Documentos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{161A4312-529B-4E5F-9B7B-5B1EA32F0D6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2BCA792-3C1F-4347-B65A-5F7CCFE25CB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1281,7 +1281,7 @@
                   <c:v>284</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>263</c:v>
+                  <c:v>226</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2358,7 +2358,7 @@
   <dimension ref="A1:M44"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2448,7 +2448,7 @@
       </c>
       <c r="K3" s="1">
         <f>SUM(K4:K8)</f>
-        <v>65</v>
+        <v>102</v>
       </c>
       <c r="L3" s="1">
         <f>J3</f>
@@ -2492,11 +2492,11 @@
         <v>13</v>
       </c>
       <c r="L4" s="1">
-        <f>L3-J4</f>
+        <f t="shared" ref="L4:M6" si="0">L3-J4</f>
         <v>315</v>
       </c>
       <c r="M4" s="1">
-        <f>M3-K4</f>
+        <f t="shared" si="0"/>
         <v>315</v>
       </c>
     </row>
@@ -2533,11 +2533,11 @@
         <v>31</v>
       </c>
       <c r="L5" s="1">
-        <f>L4-J5</f>
+        <f t="shared" si="0"/>
         <v>213</v>
       </c>
       <c r="M5" s="1">
-        <f>M4-K5</f>
+        <f t="shared" si="0"/>
         <v>284</v>
       </c>
     </row>
@@ -2559,15 +2559,15 @@
         <v>55</v>
       </c>
       <c r="K6" s="1">
-        <v>21</v>
+        <v>58</v>
       </c>
       <c r="L6" s="1">
-        <f>L5-J6</f>
+        <f t="shared" si="0"/>
         <v>158</v>
       </c>
       <c r="M6" s="1">
-        <f>M5-K6</f>
-        <v>263</v>
+        <f t="shared" si="0"/>
+        <v>226</v>
       </c>
     </row>
     <row r="7" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Muita coisa, coloquei a API web data viz, criei a função de enviar a Mensagem no entre em contato, alterei algumas coisinhas besta que não lembro...
</commit_message>
<xml_diff>
--- a/Documentos/Product-Backlog.xlsx
+++ b/Documentos/Product-Backlog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zdusa\OneDrive\Documentos\ZDU\SPTECH ZDU\1° Semestre\Projeto-Individual\Documentos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2BCA792-3C1F-4347-B65A-5F7CCFE25CB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43A7266E-1D70-4EC9-B742-AF25FBD7E88D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1281,7 +1281,7 @@
                   <c:v>284</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>226</c:v>
+                  <c:v>210</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2358,7 +2358,7 @@
   <dimension ref="A1:M44"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2448,7 +2448,7 @@
       </c>
       <c r="K3" s="1">
         <f>SUM(K4:K8)</f>
-        <v>102</v>
+        <v>118</v>
       </c>
       <c r="L3" s="1">
         <f>J3</f>
@@ -2559,7 +2559,7 @@
         <v>55</v>
       </c>
       <c r="K6" s="1">
-        <v>58</v>
+        <v>74</v>
       </c>
       <c r="L6" s="1">
         <f t="shared" si="0"/>
@@ -2567,7 +2567,7 @@
       </c>
       <c r="M6" s="1">
         <f t="shared" si="0"/>
-        <v>226</v>
+        <v>210</v>
       </c>
     </row>
     <row r="7" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Muita coisa, muita mesmo, Linkei a dash com o banco de dados, automatizei as coisas, criei um botão para salvar o jogo sempre que quiser, criei botão para sair do jogo e outro para sair da telaJogos, excluindo o sessionStorage, arrumei o sistema de classe colocando o botão para funcionar, ajeitei o sistema de nível. Comecei a passar os diálogos de combate para a tela (antes estava apenas no console). Próximos passo é fazer o perfil com conquistas.
</commit_message>
<xml_diff>
--- a/Documentos/Product-Backlog.xlsx
+++ b/Documentos/Product-Backlog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zdusa\OneDrive\Documentos\ZDU\SPTECH ZDU\1° Semestre\Projeto-Individual\Documentos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43A7266E-1D70-4EC9-B742-AF25FBD7E88D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{611091BE-A49B-4C50-868F-53D54F448835}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1282,6 +1282,9 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>210</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>134</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2358,7 +2361,7 @@
   <dimension ref="A1:M44"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+      <selection activeCell="M23" sqref="M23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2448,7 +2451,7 @@
       </c>
       <c r="K3" s="1">
         <f>SUM(K4:K8)</f>
-        <v>118</v>
+        <v>194</v>
       </c>
       <c r="L3" s="1">
         <f>J3</f>
@@ -2600,13 +2603,16 @@
         <v>121</v>
       </c>
       <c r="K7" s="1">
-        <v>0</v>
+        <v>76</v>
       </c>
       <c r="L7" s="1">
         <f>L6-J7</f>
         <v>37</v>
       </c>
-      <c r="M7" s="1"/>
+      <c r="M7" s="1">
+        <f>M6-K7</f>
+        <v>134</v>
+      </c>
     </row>
     <row r="8" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="27" t="s">

</xml_diff>

<commit_message>
Finalização do sistema de conquistas, implementado com o banco de dados, e alterações no site, além da validação de Entre em contato feita.
</commit_message>
<xml_diff>
--- a/Documentos/Product-Backlog.xlsx
+++ b/Documentos/Product-Backlog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zdusa\OneDrive\Documentos\ZDU\SPTECH ZDU\1° Semestre\Projeto-Individual\Documentos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{611091BE-A49B-4C50-868F-53D54F448835}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1279DF38-A552-4BCE-95B0-7F4DD74F51A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1285,6 +1285,9 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>134</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>121</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2361,7 +2364,7 @@
   <dimension ref="A1:M44"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="M23" sqref="M23"/>
+      <selection activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2451,7 +2454,7 @@
       </c>
       <c r="K3" s="1">
         <f>SUM(K4:K8)</f>
-        <v>194</v>
+        <v>207</v>
       </c>
       <c r="L3" s="1">
         <f>J3</f>
@@ -2492,6 +2495,7 @@
         <v>13</v>
       </c>
       <c r="K4" s="1">
+        <f>E4+E5</f>
         <v>13</v>
       </c>
       <c r="L4" s="1">
@@ -2533,6 +2537,7 @@
         <v>102</v>
       </c>
       <c r="K5" s="1">
+        <f>E7+E8+E9</f>
         <v>31</v>
       </c>
       <c r="L5" s="1">
@@ -2562,6 +2567,7 @@
         <v>55</v>
       </c>
       <c r="K6" s="1">
+        <f>E11+E12+E13+E15+E14+E16+E17+E19+E20</f>
         <v>74</v>
       </c>
       <c r="L6" s="1">
@@ -2603,6 +2609,7 @@
         <v>121</v>
       </c>
       <c r="K7" s="1">
+        <f>E21+E23+E24+E25+E27+E28+E29+E34+E36</f>
         <v>76</v>
       </c>
       <c r="L7" s="1">
@@ -2644,13 +2651,17 @@
         <v>37</v>
       </c>
       <c r="K8" s="1">
-        <v>0</v>
+        <f>E35+E37</f>
+        <v>13</v>
       </c>
       <c r="L8" s="1">
         <f>L7-J8</f>
         <v>0</v>
       </c>
-      <c r="M8" s="1"/>
+      <c r="M8" s="1">
+        <f>M7-K8</f>
+        <v>121</v>
+      </c>
     </row>
     <row r="9" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="28" t="s">

</xml_diff>